<commit_message>
Must clear code and fix dropdown elements and interaction with parent account
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Data.xlsx
+++ b/src/test/resources/testData/Data.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\selenium\Salesforce\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04E9A95-1E14-4192-86EF-59992F1D602E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9A594A98-CEB6-497D-992A-AE15399ED4A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Account Name</t>
   </si>
@@ -175,6 +171,9 @@
   </si>
   <si>
     <t>Test Description (Kamaraj Exercise!!)</t>
+  </si>
+  <si>
+    <t>11/5/2020</t>
   </si>
 </sst>
 </file>
@@ -264,10 +263,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -549,11 +548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
@@ -765,8 +764,8 @@
       <c r="AA2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="5">
-        <v>44140</v>
+      <c r="AB2" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="AC2" s="3">
         <v>123456</v>

</xml_diff>